<commit_message>
Add grades for Test 13, Test 14, and Q4 Homework / Labs average.
</commit_message>
<xml_diff>
--- a/Becky/AdvancedChemistry/Grades_Becky_Stewart_1008174.04_Advanced_Chemstry.xlsx
+++ b/Becky/AdvancedChemistry/Grades_Becky_Stewart_1008174.04_Advanced_Chemstry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5274e61be3cff2ca/Homeschool/Becky/AdvancedChemistry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="11_F25DC773A252ABDACC10487EB1DC624A5ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC19DA14-6753-4EB6-BAE8-6F7A76C0C32C}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="11_F25DC773A252ABDACC10487EB1DC624A5ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BC25DCE-FD98-419E-9A40-2197983AE655}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -484,7 +484,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,6 +746,9 @@
       <c r="A23" t="s">
         <v>19</v>
       </c>
+      <c r="B23" s="5">
+        <v>95</v>
+      </c>
       <c r="C23" s="7">
         <v>0.15</v>
       </c>
@@ -754,6 +757,9 @@
       <c r="A24" t="s">
         <v>20</v>
       </c>
+      <c r="B24" s="5">
+        <v>100</v>
+      </c>
       <c r="C24" s="7">
         <v>0.15</v>
       </c>
@@ -778,6 +784,9 @@
       <c r="A27" t="s">
         <v>28</v>
       </c>
+      <c r="B27" s="5">
+        <v>100</v>
+      </c>
       <c r="C27" s="7">
         <v>0.15</v>
       </c>
@@ -796,7 +805,7 @@
       </c>
       <c r="B29" s="5">
         <f>(B23*C23)+(B24*C24)+(B25*C25)+(B26*C26)+(B27*C27)+(B28*C28)</f>
-        <v>0</v>
+        <v>44.25</v>
       </c>
       <c r="C29" s="7">
         <f>SUM(C23:C28)</f>
@@ -809,7 +818,7 @@
       </c>
       <c r="B30" s="5">
         <f>AVERAGE(B8,B15,B22,B29)</f>
-        <v>73.837500000000006</v>
+        <v>84.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add final grades, tests, and course completion form.
</commit_message>
<xml_diff>
--- a/Becky/AdvancedChemistry/Grades_Becky_Stewart_1008174.04_Advanced_Chemstry.xlsx
+++ b/Becky/AdvancedChemistry/Grades_Becky_Stewart_1008174.04_Advanced_Chemstry.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5274e61be3cff2ca/Homeschool/Becky/AdvancedChemistry/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\celia\OneDrive\Homeschool\Becky\AdvancedChemistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="11_F25DC773A252ABDACC10487EB1DC624A5ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BC25DCE-FD98-419E-9A40-2197983AE655}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA01DA5F-7418-4D9E-AC28-6E24F3042504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Assignment</t>
   </si>
@@ -99,12 +99,6 @@
   </si>
   <si>
     <t>Test 14</t>
-  </si>
-  <si>
-    <t>Test 15</t>
-  </si>
-  <si>
-    <t>Test 16</t>
   </si>
   <si>
     <t>Quarter Test 4</t>
@@ -212,10 +206,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -481,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,10 +489,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -551,7 +541,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B6" s="5">
         <v>100</v>
@@ -630,7 +620,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B13" s="5">
         <v>100</v>
@@ -671,7 +661,7 @@
         <v>94</v>
       </c>
       <c r="C16" s="7">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -682,7 +672,7 @@
         <v>96</v>
       </c>
       <c r="C17" s="7">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -693,53 +683,53 @@
         <v>100</v>
       </c>
       <c r="C18" s="7">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="5">
+        <v>100</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="5">
+        <v>100</v>
+      </c>
+      <c r="C20" s="7">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="5">
+        <f>(B16*C16)+(B17*C17)+(B18*C18)+(B19*C19)+(B20*C20)</f>
+        <v>98</v>
+      </c>
+      <c r="C21" s="7">
+        <f>SUM(C16:C20)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="5">
-        <v>100</v>
-      </c>
-      <c r="C19" s="7">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="5">
-        <v>100</v>
-      </c>
-      <c r="C20" s="7">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="5">
-        <v>100</v>
-      </c>
-      <c r="C21" s="7">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="B22" s="5">
-        <f>(B16*C16)+(B17*C17)+(B18*C18)+(B19*C19)+(B20*C20)+(B21*C21)</f>
-        <v>98.5</v>
+        <v>100</v>
       </c>
       <c r="C22" s="7">
-        <f>SUM(C16:C21)</f>
-        <v>1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -750,7 +740,7 @@
         <v>95</v>
       </c>
       <c r="C23" s="7">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -761,64 +751,51 @@
         <v>100</v>
       </c>
       <c r="C24" s="7">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="5">
+        <v>100</v>
+      </c>
+      <c r="C25" s="7">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="7">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B26" s="5">
+        <v>88</v>
+      </c>
+      <c r="C26" s="7">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="7">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>28</v>
-      </c>
       <c r="B27" s="5">
-        <v>100</v>
+        <f>(B22*C22)+(B23*C23)+(B24*C24)+(B25*C25)+(B26*C26)</f>
+        <v>96</v>
       </c>
       <c r="C27" s="7">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+        <f>SUM(C22:C26)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A28" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="7">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="5">
-        <f>(B23*C23)+(B24*C24)+(B25*C25)+(B26*C26)+(B27*C27)+(B28*C28)</f>
-        <v>44.25</v>
-      </c>
-      <c r="C29" s="7">
-        <f>SUM(C23:C28)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A30" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="5">
-        <f>AVERAGE(B8,B15,B22,B29)</f>
-        <v>84.9</v>
+      <c r="B28" s="5">
+        <f>AVERAGE(B8,B15,B21,B27)</f>
+        <v>97.712500000000006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>